<commit_message>
Last version of the Notebook
</commit_message>
<xml_diff>
--- a/Reports_Insight_Tables/Model_Selection.xlsx
+++ b/Reports_Insight_Tables/Model_Selection.xlsx
@@ -1,20 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e621d9677247b745/Data_26-07/Water_Potability/Reports_Insight_Tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_FBBE4426BE31921FD2FE31D2F8F2D3C274D88D68" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB2B6CA8-5B77-4999-921B-BD104DDB1924}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Accuray</t>
   </si>
@@ -53,13 +71,37 @@
   </si>
   <si>
     <t>Logistic</t>
+  </si>
+  <si>
+    <t>tree_QT</t>
+  </si>
+  <si>
+    <t>Tree_MM</t>
+  </si>
+  <si>
+    <t>tree_RS</t>
+  </si>
+  <si>
+    <t>tree_PT</t>
+  </si>
+  <si>
+    <t>Tree_SC</t>
+  </si>
+  <si>
+    <t>tree_PL</t>
+  </si>
+  <si>
+    <t>tree_MA</t>
+  </si>
+  <si>
+    <t>tree_N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +164,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -168,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,9 +250,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,6 +302,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,14 +495,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="A20:G20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,12 +530,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C2">
         <v>0.43</v>
@@ -456,15 +550,15 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0.55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C3">
         <v>0.43</v>
@@ -479,10 +573,10 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -505,7 +599,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -528,7 +622,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -551,7 +645,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -559,7 +653,7 @@
         <v>0.64</v>
       </c>
       <c r="C7">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D7">
         <v>0.3</v>
@@ -574,7 +668,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -595,6 +689,210 @@
       </c>
       <c r="G8">
         <v>0.61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C15">
+        <v>0.45</v>
+      </c>
+      <c r="D15">
+        <v>0.48</v>
+      </c>
+      <c r="E15">
+        <v>0.46</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C16">
+        <v>0.43</v>
+      </c>
+      <c r="D16">
+        <v>0.47</v>
+      </c>
+      <c r="E16">
+        <v>0.45</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.54</v>
+      </c>
+      <c r="C17">
+        <v>0.42</v>
+      </c>
+      <c r="D17">
+        <v>0.47</v>
+      </c>
+      <c r="E17">
+        <v>0.45</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C18">
+        <v>0.44</v>
+      </c>
+      <c r="D18">
+        <v>0.46</v>
+      </c>
+      <c r="E18">
+        <v>0.45</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C19">
+        <v>0.43</v>
+      </c>
+      <c r="D19">
+        <v>0.45</v>
+      </c>
+      <c r="E19">
+        <v>0.44</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C20">
+        <v>0.47</v>
+      </c>
+      <c r="D20">
+        <v>0.45</v>
+      </c>
+      <c r="E20">
+        <v>0.46</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C21">
+        <v>0.43</v>
+      </c>
+      <c r="D21">
+        <v>0.44</v>
+      </c>
+      <c r="E21">
+        <v>0.43</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C22">
+        <v>0.42</v>
+      </c>
+      <c r="D22">
+        <v>0.38</v>
+      </c>
+      <c r="E22">
+        <v>0.4</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>